<commit_message>
Almost ready to fabricate PCB. I need to do one last look over, concentrating on schematic.
</commit_message>
<xml_diff>
--- a/cyclops_r3/parts/cyclops_r3-5.xlsx
+++ b/cyclops_r3/parts/cyclops_r3-5.xlsx
@@ -433,7 +433,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,14 +573,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -960,7 +952,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1003,14 +995,12 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="14" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="7" applyBorder="1"/>
@@ -1029,7 +1019,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1063,7 +1053,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1353,10 +1342,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1353,7 @@
     <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.140625" style="13" customWidth="1"/>
+    <col min="5" max="6" width="10.140625" style="12" customWidth="1"/>
     <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.28515625" bestFit="1" customWidth="1"/>
@@ -1383,1332 +1372,1332 @@
       <c r="D1" t="s">
         <v>119</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="13">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13" t="s">
+      <c r="B2" s="12">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>7</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <f>G2/B2</f>
         <v>7</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <f xml:space="preserve"> IF(3*B2 -G2 &gt; 0, CEILING(3*B2 -G2, 1), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="B3" s="12">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
         <f>G3/B3</f>
         <v>0</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <f xml:space="preserve"> IF(3*B3 -G3 &gt; 0, CEILING(3*B3 -G3, 1), 0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>13</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>100</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f>G4/B4</f>
         <v>7.6923076923076925</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <f t="shared" ref="I4:I66" si="0" xml:space="preserve"> IF(3*B4 -G4 &gt; 0, CEILING(3*B4 -G4, 1), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="13">
-        <v>1</v>
-      </c>
-      <c r="C5" s="13" t="s">
+      <c r="B5" s="12">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
         <f>G5/B5</f>
         <v>0</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>5</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>45</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f>G6/B6</f>
         <v>9</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="13">
-        <v>1</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B7" s="12">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
         <f>G7/B7</f>
         <v>0</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>4</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>8</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f>G8/B8</f>
         <v>2</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="13">
-        <v>1</v>
-      </c>
-      <c r="C9" s="13" t="s">
+      <c r="B9" s="12">
+        <v>1</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>7</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f>G9/B9</f>
         <v>7</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="5">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="3">
         <f>G10/B10</f>
         <v>0</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="B11" s="13">
-        <v>1</v>
-      </c>
-      <c r="C11" s="13" t="s">
+      <c r="B11" s="12">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="G11" s="5">
-        <v>0</v>
-      </c>
-      <c r="H11" s="4">
+      <c r="G11" s="4">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
         <f>G11/B11</f>
         <v>0</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="13">
-        <v>2</v>
-      </c>
-      <c r="C12" s="13" t="s">
+      <c r="B12" s="12">
+        <v>2</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>15</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f>G12/B12</f>
         <v>7.5</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="13" t="s">
+      <c r="B13" s="12">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="5">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="G13" s="4">
+        <v>0</v>
+      </c>
+      <c r="H13" s="3">
         <f>G13/B13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="13">
-        <v>2</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="12">
+        <v>2</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="5">
-        <v>0</v>
-      </c>
-      <c r="H14" s="4">
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
         <f>G14/B14</f>
         <v>0</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B15" s="13">
-        <v>2</v>
-      </c>
-      <c r="C15" s="13" t="s">
+      <c r="B15" s="12">
+        <v>2</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="5">
-        <v>0</v>
-      </c>
-      <c r="H15" s="4">
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
         <f>G15/B15</f>
         <v>0</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="13">
-        <v>1</v>
-      </c>
-      <c r="C16" s="13" t="s">
+      <c r="B16" s="12">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <v>10</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <f>G16/B16</f>
         <v>10</v>
       </c>
-      <c r="I16" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="I16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="B17" s="13">
-        <v>1</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="B17" s="12">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>10</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <f>G17/B17</f>
         <v>10</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="13">
-        <v>1</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="B18" s="12">
+        <v>1</v>
+      </c>
+      <c r="C18" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <v>20</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <f>G18/B18</f>
         <v>20</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="13">
-        <v>1</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="B19" s="12">
+        <v>1</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="G19" s="5">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="3">
         <f>G19/B19</f>
         <v>0</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="13">
-        <v>2</v>
-      </c>
-      <c r="C20" s="13" t="s">
+      <c r="B20" s="12">
+        <v>2</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>4</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f>G20/B20</f>
         <v>2</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="13">
-        <v>1</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="12">
+        <v>1</v>
+      </c>
+      <c r="C21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>4</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <f>G21/B21</f>
         <v>4</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="13">
-        <v>1</v>
-      </c>
-      <c r="C22" s="13" t="s">
+      <c r="B22" s="12">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="5">
-        <v>2</v>
-      </c>
-      <c r="H22" s="4">
+      <c r="G22" s="4">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3">
         <f>G22/B22</f>
         <v>2</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="13">
-        <v>1</v>
-      </c>
-      <c r="C23" s="13" t="s">
+      <c r="B23" s="12">
+        <v>1</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="5">
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="3">
         <f>G23/B23</f>
         <v>0</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="13">
+      <c r="B24" s="12">
         <v>7</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <v>20</v>
       </c>
-      <c r="H24" s="4">
+      <c r="H24" s="3">
         <f>G24/B24</f>
         <v>2.8571428571428572</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="13">
-        <v>1</v>
-      </c>
-      <c r="C25" s="13" t="s">
+      <c r="B25" s="12">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="G25" s="5">
-        <v>0</v>
-      </c>
-      <c r="H25" s="4">
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="3">
         <f>G25/B25</f>
         <v>0</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B26" s="13">
-        <v>1</v>
-      </c>
-      <c r="C26" s="13" t="s">
+      <c r="B26" s="12">
+        <v>1</v>
+      </c>
+      <c r="C26" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4">
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="3">
         <f>G26/B26</f>
         <v>0</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="13">
-        <v>1</v>
-      </c>
-      <c r="C27" s="13" t="s">
+      <c r="B27" s="12">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <v>9</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <f>G27/B27</f>
         <v>9</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="13">
-        <v>1</v>
-      </c>
-      <c r="C28" s="13" t="s">
+      <c r="B28" s="12">
+        <v>1</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="4">
         <v>8</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H28" s="3">
         <f>G28/B28</f>
         <v>8</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="13">
-        <v>1</v>
-      </c>
-      <c r="C29" s="13" t="s">
+      <c r="B29" s="12">
+        <v>1</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="4">
         <v>6</v>
       </c>
-      <c r="H29" s="4">
+      <c r="H29" s="3">
         <f>G29/B29</f>
         <v>6</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="13">
+      <c r="B30" s="12">
         <v>7</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="4">
         <v>50</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="3">
         <f>G30/B30</f>
         <v>7.1428571428571432</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B31" s="13">
-        <v>1</v>
-      </c>
-      <c r="C31" s="13" t="s">
+      <c r="B31" s="12">
+        <v>1</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
-      <c r="H31" s="4">
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="3">
         <f>G31/B31</f>
         <v>0</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="13">
-        <v>1</v>
-      </c>
-      <c r="C32" s="13" t="s">
+      <c r="B32" s="12">
+        <v>1</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G32" s="5">
-        <v>0</v>
-      </c>
-      <c r="H32" s="4">
+      <c r="G32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="3">
         <f>G32/B32</f>
         <v>0</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="13">
-        <v>1</v>
-      </c>
-      <c r="C33" s="13" t="s">
+      <c r="B33" s="12">
+        <v>1</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G33" s="5">
-        <v>0</v>
-      </c>
-      <c r="H33" s="4">
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="3">
         <f>G33/B33</f>
         <v>0</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="2">
         <f xml:space="preserve"> IF(3*B33 -G33 &gt; 0, CEILING(3*B33 -G33, 1), 0)</f>
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="13">
-        <v>1</v>
-      </c>
-      <c r="C34" s="13" t="s">
+      <c r="B34" s="12">
+        <v>1</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G34" s="5">
-        <v>0</v>
-      </c>
-      <c r="H34" s="4">
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
         <f>G34/B34</f>
         <v>0</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="13">
-        <v>2</v>
-      </c>
-      <c r="C35" s="13" t="s">
+      <c r="B35" s="12">
+        <v>2</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G35" s="5">
-        <v>0</v>
-      </c>
-      <c r="H35" s="4">
+      <c r="G35" s="4">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
         <f>G35/B35</f>
         <v>0</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="13">
-        <v>1</v>
-      </c>
-      <c r="C36" s="13" t="s">
+      <c r="B36" s="12">
+        <v>1</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G36" s="5">
-        <v>0</v>
-      </c>
-      <c r="H36" s="4">
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
         <f>G36/B36</f>
         <v>0</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="13">
+      <c r="B37" s="12">
         <v>8</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G37" s="5">
+      <c r="G37" s="4">
         <v>100</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="3">
         <f>G37/B37</f>
         <v>12.5</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="13">
-        <v>2</v>
-      </c>
-      <c r="C38" s="13" t="s">
+      <c r="B38" s="12">
+        <v>2</v>
+      </c>
+      <c r="C38" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="4">
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
         <f>G38/B38</f>
         <v>0</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="13">
-        <v>1</v>
-      </c>
-      <c r="C39" s="13" t="s">
+      <c r="B39" s="12">
+        <v>1</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="4">
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="3">
         <f>G39/B39</f>
         <v>0</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="13">
-        <v>2</v>
-      </c>
-      <c r="C40" s="13" t="s">
+      <c r="B40" s="12">
+        <v>2</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G40" s="5">
+      <c r="G40" s="4">
         <v>40</v>
       </c>
-      <c r="H40" s="4">
+      <c r="H40" s="3">
         <f>G40/B40</f>
         <v>20</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="12">
         <v>3</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G41" s="5">
-        <v>0</v>
-      </c>
-      <c r="H41" s="4">
+      <c r="G41" s="4">
+        <v>0</v>
+      </c>
+      <c r="H41" s="3">
         <f>G41/B41</f>
         <v>0</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="13">
-        <v>2</v>
-      </c>
-      <c r="C42" s="13" t="s">
+      <c r="B42" s="12">
+        <v>2</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G42" s="5">
-        <v>0</v>
-      </c>
-      <c r="H42" s="4">
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
         <f>G42/B42</f>
         <v>0</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="A43" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B43" s="13">
-        <v>1</v>
-      </c>
-      <c r="C43" s="13" t="s">
+      <c r="B43" s="12">
+        <v>1</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G43" s="4">
         <v>5</v>
       </c>
-      <c r="H43" s="4">
+      <c r="H43" s="3">
         <f>G43/B43</f>
         <v>5</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="13">
-        <v>1</v>
-      </c>
-      <c r="C44" s="13" t="s">
+      <c r="B44" s="12">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G44" s="5">
-        <v>0</v>
-      </c>
-      <c r="H44" s="4">
+      <c r="G44" s="4">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
         <f>G44/B44</f>
         <v>0</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="A45" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="13">
-        <v>1</v>
-      </c>
-      <c r="C45" s="13" t="s">
+      <c r="B45" s="12">
+        <v>1</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="G45" s="5">
-        <v>2</v>
-      </c>
-      <c r="H45" s="4">
+      <c r="G45" s="4">
+        <v>2</v>
+      </c>
+      <c r="H45" s="3">
         <f>G45/B45</f>
         <v>2</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="12">
         <v>6</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="G46" s="5">
+      <c r="G46" s="4">
         <v>9</v>
       </c>
-      <c r="H46" s="4">
+      <c r="H46" s="3">
         <f>G46/B46</f>
         <v>1.5</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="A47" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="13">
-        <v>1</v>
-      </c>
-      <c r="C47" s="13" t="s">
+      <c r="B47" s="12">
+        <v>1</v>
+      </c>
+      <c r="C47" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="G47" s="5">
-        <v>2</v>
-      </c>
-      <c r="H47" s="4">
+      <c r="G47" s="4">
+        <v>2</v>
+      </c>
+      <c r="H47" s="3">
         <f>G47/B47</f>
         <v>2</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="13">
-        <v>1</v>
-      </c>
-      <c r="C48" s="13" t="s">
+      <c r="B48" s="12">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="4">
         <v>5</v>
       </c>
-      <c r="H48" s="4">
+      <c r="H48" s="3">
         <f>G48/B48</f>
         <v>5</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B49" s="13">
-        <v>1</v>
-      </c>
-      <c r="C49" s="13" t="s">
+      <c r="B49" s="12">
+        <v>1</v>
+      </c>
+      <c r="C49" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G49" s="5">
+      <c r="G49" s="4">
         <v>4</v>
       </c>
-      <c r="H49" s="4">
+      <c r="H49" s="3">
         <f>G49/B49</f>
         <v>4</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B50" s="13">
-        <v>1</v>
-      </c>
-      <c r="C50" s="13" t="s">
+      <c r="B50" s="12">
+        <v>1</v>
+      </c>
+      <c r="C50" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G50" s="5">
-        <v>0</v>
-      </c>
-      <c r="H50" s="4">
+      <c r="G50" s="4">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
         <f>G50/B50</f>
         <v>0</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="13">
-        <v>1</v>
-      </c>
-      <c r="C51" s="13" t="s">
+      <c r="B51" s="12">
+        <v>1</v>
+      </c>
+      <c r="C51" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="G51" s="5">
+      <c r="G51" s="4">
         <v>7</v>
       </c>
-      <c r="H51" s="4">
+      <c r="H51" s="3">
         <f>G51/B51</f>
         <v>7</v>
       </c>
-      <c r="I51" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="I51" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B52" s="13">
-        <v>1</v>
-      </c>
-      <c r="C52" s="13" t="s">
+      <c r="B52" s="12">
+        <v>1</v>
+      </c>
+      <c r="C52" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G52" s="5">
-        <v>0</v>
-      </c>
-      <c r="H52" s="4">
+      <c r="G52" s="4">
+        <v>0</v>
+      </c>
+      <c r="H52" s="3">
         <f>G52/B52</f>
         <v>0</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B53" s="13">
-        <v>1</v>
-      </c>
-      <c r="C53" s="13" t="s">
+      <c r="B53" s="12">
+        <v>1</v>
+      </c>
+      <c r="C53" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G53" s="5">
+      <c r="G53" s="4">
         <v>7</v>
       </c>
-      <c r="H53" s="4">
+      <c r="H53" s="3">
         <f>G53/B53</f>
         <v>7</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="B54" s="13">
-        <v>1</v>
-      </c>
-      <c r="C54" s="13" t="s">
+      <c r="B54" s="12">
+        <v>1</v>
+      </c>
+      <c r="C54" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="G54" s="5">
-        <v>2</v>
-      </c>
-      <c r="H54" s="4">
+      <c r="G54" s="4">
+        <v>2</v>
+      </c>
+      <c r="H54" s="3">
         <f>G54/B54</f>
         <v>2</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="13">
-        <v>1</v>
-      </c>
-      <c r="C55" s="13" t="s">
+      <c r="B55" s="12">
+        <v>1</v>
+      </c>
+      <c r="C55" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="G55" s="5">
-        <v>1</v>
-      </c>
-      <c r="H55" s="4">
+      <c r="G55" s="4">
+        <v>1</v>
+      </c>
+      <c r="H55" s="3">
         <f>G55/B55</f>
         <v>1</v>
       </c>
-      <c r="I55" s="3">
+      <c r="I55" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B56" s="13">
-        <v>1</v>
-      </c>
-      <c r="C56" s="13" t="s">
+      <c r="B56" s="12">
+        <v>1</v>
+      </c>
+      <c r="C56" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="5">
+      <c r="G56" s="4">
         <v>4</v>
       </c>
-      <c r="H56" s="4">
+      <c r="H56" s="3">
         <f>G56/B56</f>
         <v>4</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B57" s="13">
-        <v>1</v>
-      </c>
-      <c r="C57" s="13" t="s">
+      <c r="B57" s="12">
+        <v>1</v>
+      </c>
+      <c r="C57" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="G57" s="5">
-        <v>0</v>
-      </c>
-      <c r="H57" s="4">
+      <c r="G57" s="4">
+        <v>0</v>
+      </c>
+      <c r="H57" s="3">
         <f>G57/B57</f>
         <v>0</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="B58" s="13">
-        <v>1</v>
-      </c>
-      <c r="C58" s="13" t="s">
+      <c r="B58" s="12">
+        <v>1</v>
+      </c>
+      <c r="C58" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="G58" s="5">
-        <v>1</v>
-      </c>
-      <c r="H58" s="4">
+      <c r="G58" s="4">
+        <v>1</v>
+      </c>
+      <c r="H58" s="3">
         <f>G58/B58</f>
         <v>1</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B59" s="13">
-        <v>2</v>
-      </c>
-      <c r="C59" s="13" t="s">
+      <c r="B59" s="12">
+        <v>2</v>
+      </c>
+      <c r="C59" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="G59" s="5">
+      <c r="G59" s="4">
         <v>4</v>
       </c>
-      <c r="H59" s="4">
+      <c r="H59" s="3">
         <f>G59/B59</f>
         <v>2</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59" s="2">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+      <c r="A60" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B60" s="13">
-        <v>1</v>
-      </c>
-      <c r="C60" s="13" t="s">
+      <c r="B60" s="12">
+        <v>1</v>
+      </c>
+      <c r="C60" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="G60" s="5">
+      <c r="G60" s="4">
         <v>4</v>
       </c>
-      <c r="H60" s="4">
+      <c r="H60" s="3">
         <f>G60/B60</f>
         <v>4</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+      <c r="A61" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B61" s="13">
+      <c r="B61" s="12">
         <v>3</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="C61" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="G61" s="5">
+      <c r="G61" s="4">
         <v>8</v>
       </c>
-      <c r="H61" s="4">
+      <c r="H61" s="3">
         <f>G61/B61</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="I61" s="3">
+      <c r="I61" s="2">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2723,14 +2712,14 @@
       <c r="C62" t="s">
         <v>58</v>
       </c>
-      <c r="G62" s="5">
+      <c r="G62" s="4">
         <v>9</v>
       </c>
-      <c r="H62" s="4">
+      <c r="H62" s="3">
         <f>G62/B62</f>
         <v>9</v>
       </c>
-      <c r="I62" s="3">
+      <c r="I62" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2745,20 +2734,20 @@
       <c r="C63" t="s">
         <v>60</v>
       </c>
-      <c r="G63" s="5">
-        <v>1</v>
-      </c>
-      <c r="H63" s="4">
+      <c r="G63" s="4">
+        <v>1</v>
+      </c>
+      <c r="H63" s="3">
         <f>G63/B63</f>
         <v>1</v>
       </c>
-      <c r="I63" s="3">
+      <c r="I63" s="2">
         <f xml:space="preserve"> IF(3*B63 -G63 &gt; 0, CEILING(3*B63 -G63, 1), 0)</f>
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="12" t="s">
         <v>134</v>
       </c>
       <c r="B64">
@@ -2767,39 +2756,39 @@
       <c r="C64" t="s">
         <v>111</v>
       </c>
-      <c r="G64" s="5">
-        <v>0</v>
-      </c>
-      <c r="H64" s="4">
+      <c r="G64" s="4">
+        <v>0</v>
+      </c>
+      <c r="H64" s="3">
         <f>G64/B64</f>
         <v>0</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I64" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="12" t="s">
         <v>112</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
-      <c r="C65" s="9" t="s">
+      <c r="C65" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D65" s="13" t="s">
+      <c r="D65" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G65" s="5">
-        <v>0</v>
-      </c>
-      <c r="H65" s="4">
+      <c r="G65" s="4">
+        <v>0</v>
+      </c>
+      <c r="H65" s="3">
         <f>G65/B65</f>
         <v>0</v>
       </c>
-      <c r="I65" s="3">
+      <c r="I65" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
@@ -2817,193 +2806,176 @@
       <c r="D66" t="s">
         <v>118</v>
       </c>
-      <c r="G66" s="5">
-        <v>1</v>
-      </c>
-      <c r="H66" s="4">
+      <c r="G66" s="4">
+        <v>1</v>
+      </c>
+      <c r="H66" s="3">
         <f>G66/B66</f>
         <v>1</v>
       </c>
-      <c r="I66" s="3">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G67" s="5"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="3"/>
+      <c r="I66" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G67" s="4"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="2"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>61</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1</v>
-      </c>
-      <c r="C68" t="s">
-        <v>2</v>
-      </c>
-      <c r="D68" t="s">
-        <v>119</v>
-      </c>
-      <c r="G68" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H68" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I68" s="3"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="2"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>119</v>
+      </c>
+      <c r="G69" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I69" s="2"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>70</v>
       </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
         <v>116</v>
       </c>
-      <c r="G69" s="5">
-        <v>0</v>
-      </c>
-      <c r="H69" s="4">
-        <f>G69/B69</f>
-        <v>0</v>
-      </c>
-      <c r="I69" s="3">
-        <f t="shared" ref="I69" si="1" xml:space="preserve"> IF(3*B69 -G69 &gt; 0, CEILING(3*B69 -G69, 1), 0)</f>
+      <c r="G70" s="4">
+        <v>0</v>
+      </c>
+      <c r="H70" s="3">
+        <f>G70/B70</f>
+        <v>0</v>
+      </c>
+      <c r="I70" s="2">
+        <f t="shared" ref="I70" si="1" xml:space="preserve"> IF(3*B70 -G70 &gt; 0, CEILING(3*B70 -G70, 1), 0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G70" s="5"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="3"/>
-    </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="G71" s="4"/>
+      <c r="H71" s="3"/>
+      <c r="I71" s="2"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>62</v>
       </c>
-      <c r="B71" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D71" s="13" t="s">
+      <c r="B72" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C72" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D72" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="G72" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="H71" s="4" t="s">
+      <c r="H72" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="I71" s="3"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
-        <v>849</v>
-      </c>
-      <c r="B72">
-        <v>1</v>
-      </c>
-      <c r="C72" t="s">
-        <v>132</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G72" s="5">
-        <v>1</v>
-      </c>
-      <c r="H72" s="4">
-        <f>G72/B72</f>
-        <v>1</v>
-      </c>
-      <c r="I72" s="3">
-        <f t="shared" ref="I72:I73" si="2" xml:space="preserve"> IF(3*B72 -G72 &gt; 0, CEILING(3*B72 -G72, 1), 0)</f>
-        <v>2</v>
-      </c>
+      <c r="I72" s="2"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
+        <v>849</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73" t="s">
+        <v>132</v>
+      </c>
+      <c r="D73" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G73" s="4">
+        <v>1</v>
+      </c>
+      <c r="H73" s="3">
+        <f>G73/B73</f>
+        <v>1</v>
+      </c>
+      <c r="I73" s="2">
+        <f t="shared" ref="I73:I74" si="2" xml:space="preserve"> IF(3*B73 -G73 &gt; 0, CEILING(3*B73 -G73, 1), 0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
         <v>85</v>
       </c>
-      <c r="B73">
-        <v>1</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74" t="s">
         <v>71</v>
       </c>
-      <c r="D73" s="13" t="s">
+      <c r="D74" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G73" s="5">
-        <v>0</v>
-      </c>
-      <c r="H73" s="4">
-        <f>G73/B73</f>
-        <v>0</v>
-      </c>
-      <c r="I73" s="3">
+      <c r="G74" s="4">
+        <v>0</v>
+      </c>
+      <c r="H74" s="3">
+        <f>G74/B74</f>
+        <v>0</v>
+      </c>
+      <c r="I74" s="2">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G74" s="5"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="3"/>
-    </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>63</v>
-      </c>
-      <c r="B75" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D75" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G75" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H75" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I75" s="3"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="2"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>64</v>
-      </c>
-      <c r="B76">
-        <v>1</v>
-      </c>
-      <c r="C76" t="s">
-        <v>72</v>
-      </c>
-      <c r="G76" s="5">
-        <v>9</v>
-      </c>
-      <c r="H76" s="4">
-        <f>G76/B76</f>
-        <v>9</v>
-      </c>
-      <c r="I76" s="3">
-        <f t="shared" ref="I76:I78" si="3" xml:space="preserve"> IF(3*B76 -G76 &gt; 0, CEILING(3*B76 -G76, 1), 0)</f>
-        <v>0</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C76" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I76" s="2"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -3011,161 +2983,179 @@
       <c r="C77" t="s">
         <v>72</v>
       </c>
-      <c r="G77" s="5">
+      <c r="G77" s="4">
         <v>9</v>
       </c>
-      <c r="H77" s="4">
-        <f t="shared" ref="H77:H78" si="4">G77/B77</f>
+      <c r="H77" s="3">
+        <f>G77/B77</f>
         <v>9</v>
       </c>
-      <c r="I77" s="3">
-        <f t="shared" si="3"/>
+      <c r="I77" s="2">
+        <f t="shared" ref="I77:I79" si="3" xml:space="preserve"> IF(3*B77 -G77 &gt; 0, CEILING(3*B77 -G77, 1), 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>65</v>
+      </c>
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>72</v>
+      </c>
+      <c r="G78" s="4">
+        <v>9</v>
+      </c>
+      <c r="H78" s="3">
+        <f t="shared" ref="H78:H79" si="4">G78/B78</f>
+        <v>9</v>
+      </c>
+      <c r="I78" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>66</v>
       </c>
-      <c r="B78">
-        <v>1</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
         <v>120</v>
       </c>
-      <c r="D78" s="13" t="s">
+      <c r="D79" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G78" s="5">
-        <v>2</v>
-      </c>
-      <c r="H78" s="4">
+      <c r="G79" s="4">
+        <v>2</v>
+      </c>
+      <c r="H79" s="3">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="I78" s="3">
+      <c r="I79" s="2">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G79" s="5"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="3"/>
-    </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>67</v>
-      </c>
-      <c r="B80" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C80" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D80" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G80" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H80" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I80" s="3"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="2"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>67</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C81" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I81" s="2"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>69</v>
       </c>
-      <c r="B81">
-        <v>1</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="B82">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
         <v>68</v>
       </c>
-      <c r="D81" s="13" t="s">
+      <c r="D82" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G81" s="5">
-        <v>0</v>
-      </c>
-      <c r="H81" s="4">
-        <f>G81/B81</f>
-        <v>0</v>
-      </c>
-      <c r="I81" s="3">
-        <f t="shared" ref="I81" si="5" xml:space="preserve"> IF(3*B81 -G81 &gt; 0, CEILING(3*B81 -G81, 1), 0)</f>
+      <c r="G82" s="4">
+        <v>0</v>
+      </c>
+      <c r="H82" s="3">
+        <f>G82/B82</f>
+        <v>0</v>
+      </c>
+      <c r="I82" s="2">
+        <f t="shared" ref="I82" si="5" xml:space="preserve"> IF(3*B82 -G82 &gt; 0, CEILING(3*B82 -G82, 1), 0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G82" s="5"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="3"/>
-    </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>114</v>
-      </c>
-      <c r="B83" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D83" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G83" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H83" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I83" s="3"/>
+      <c r="G83" s="4"/>
+      <c r="H83" s="3"/>
+      <c r="I83" s="2"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>114</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C84" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I84" s="2"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>115</v>
       </c>
-      <c r="B84">
-        <v>1</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="B85">
+        <v>1</v>
+      </c>
+      <c r="C85" t="s">
         <v>116</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="D85" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="G84" s="5">
-        <v>0</v>
-      </c>
-      <c r="H84" s="4">
-        <f>G84/B84</f>
-        <v>0</v>
-      </c>
-      <c r="I84" s="3">
-        <f t="shared" ref="I84" si="6" xml:space="preserve"> IF(3*B84 -G84 &gt; 0, CEILING(3*B84 -G84, 1), 0)</f>
+      <c r="G85" s="4">
+        <v>0</v>
+      </c>
+      <c r="H85" s="3">
+        <f>G85/B85</f>
+        <v>0</v>
+      </c>
+      <c r="I85" s="2">
+        <f t="shared" ref="I85" si="6" xml:space="preserve"> IF(3*B85 -G85 &gt; 0, CEILING(3*B85 -G85, 1), 0)</f>
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G85" s="12" t="s">
+    <row r="86" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G86" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="H85" s="11"/>
-      <c r="I85" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G85:I85"/>
+    <mergeCell ref="G86:I86"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A64" r:id="rId1" display="http://www.digikey.com/product-detail/en/AFM60US15/1470-1017-ND/4487398"/>
-    <hyperlink ref="A65" r:id="rId2" display="http://www.digikey.com/product-detail/en/SRB22A2FBRNN/CH761-ND/446027"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" fitToHeight="0" orientation="portrait" r:id="rId3"/>
+  <pageSetup scale="56" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>